<commit_message>
Moddification of the 0.9 alfa to 0.5. It's not included the 0.2 alfa and replaced with 0.5 one.
</commit_message>
<xml_diff>
--- a/bip1271_015_data.xlsx
+++ b/bip1271_015_data.xlsx
@@ -296,6 +296,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Croston's and Exponential Smoothing forecasts of item BIP001271, alpha = 0.15</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2509,13 +2539,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
+      <xdr:colOff>495298</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>2981324</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
@@ -2828,8 +2858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29:P38"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modifications to the resulting data
</commit_message>
<xml_diff>
--- a/bip1271_015_data.xlsx
+++ b/bip1271_015_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>X</t>
   </si>
@@ -199,15 +199,15 @@
   </si>
   <si>
     <t>MAE variation</t>
+  </si>
+  <si>
+    <t>Error size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000%"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,7 +262,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2856,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3937,7 +3941,7 @@
         <v>15.774134</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3968,21 +3972,24 @@
       <c r="J33">
         <v>15.363199038699481</v>
       </c>
-      <c r="L33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4">
-        <f>(M32-N32)/N32</f>
-        <v>8.2792442473829816E-2</v>
-      </c>
-      <c r="O33" s="4">
-        <f>(M32-O32)/O32</f>
-        <v>8.422801533115841E-2</v>
-      </c>
-      <c r="P33" s="4">
-        <f>(M32-P32)/P32</f>
-        <v>8.4516081833715909E-2</v>
+      <c r="L33" t="s">
+        <v>60</v>
+      </c>
+      <c r="M33" s="2">
+        <f>M32-M31</f>
+        <v>3.4510909999999999</v>
+      </c>
+      <c r="N33" s="2">
+        <f>N32-N31</f>
+        <v>3.5427490000000006</v>
+      </c>
+      <c r="O33" s="2">
+        <f>O32-O31</f>
+        <v>3.7321270000000002</v>
+      </c>
+      <c r="P33" s="2">
+        <f>P32-P31</f>
+        <v>3.7377500000000001</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4016,17 +4023,13 @@
       <c r="J34">
         <v>-14.94128081710544</v>
       </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4">
-        <f>(N32-O32)/O32</f>
-        <v>1.3258061296113018E-3</v>
-      </c>
-      <c r="P34" s="4">
-        <f>(N32-P32)/P32</f>
-        <v>1.5918465000994504E-3</v>
-      </c>
+      <c r="L34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -4059,16 +4062,24 @@
       <c r="J35">
         <v>-12.70008869453962</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4">
-        <f>(O32-P32)/P32</f>
-        <v>2.6568811955068341E-4</v>
+      <c r="L35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5">
+        <f>(M32-N32)/N32</f>
+        <v>8.2792442473829816E-2</v>
+      </c>
+      <c r="O35" s="5">
+        <f>(M32-O32)/O32</f>
+        <v>8.422801533115841E-2</v>
+      </c>
+      <c r="P35" s="5">
+        <f>(M32-P32)/P32</f>
+        <v>8.4516081833715909E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -4099,20 +4110,21 @@
       <c r="J36">
         <v>30.204924609641321</v>
       </c>
-      <c r="L36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N36" s="4">
-        <f>(M31-N31)/N31</f>
-        <v>0.11420198025618267</v>
-      </c>
-      <c r="O36" s="4">
-        <f>(M31-O31)/O31</f>
-        <v>0.13365320742694087</v>
-      </c>
-      <c r="P36" s="4">
-        <f>(M31-P31)/P31</f>
-        <v>0.1345775442192606</v>
+      <c r="L36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M36" s="5">
+        <f>(N32-M32)/M32</f>
+        <v>-7.6461969280720063E-2</v>
+      </c>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5">
+        <f>(N32-O32)/O32</f>
+        <v>1.3258061296113018E-3</v>
+      </c>
+      <c r="P36" s="5">
+        <f>(N32-P32)/P32</f>
+        <v>1.5918465000994504E-3</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -4146,14 +4158,21 @@
       <c r="J37">
         <v>44.674185918195121</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="O37" s="4">
-        <f>(N31-O31)/O31</f>
-        <v>1.7457541375295246E-2</v>
-      </c>
-      <c r="P37" s="4">
-        <f>(N31-P31)/P31</f>
-        <v>1.82871367347535E-2</v>
+      <c r="L37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M37" s="5">
+        <f>(O32-M32)/M32</f>
+        <v>-7.7684780452230276E-2</v>
+      </c>
+      <c r="N37" s="5">
+        <f>(O32-N32)/N32</f>
+        <v>-1.3240506950838436E-3</v>
+      </c>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5">
+        <f>(O32-P32)/P32</f>
+        <v>2.6568811955068341E-4</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4172,11 +4191,22 @@
       <c r="F38">
         <v>18.380500000000001</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="P38" s="4">
-        <f>(O31-P31)/P31</f>
-        <v>8.1536115830139956E-4</v>
-      </c>
+      <c r="L38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M38" s="5">
+        <f>(P32-M32)/M32</f>
+        <v>-7.7929763559443824E-2</v>
+      </c>
+      <c r="N38" s="5">
+        <f>(P32-N32)/N32</f>
+        <v>-1.5893165521084264E-3</v>
+      </c>
+      <c r="O38" s="5">
+        <f>(P32-O32)/O32</f>
+        <v>-2.6561754812380275E-4</v>
+      </c>
+      <c r="P38" s="4"/>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -4194,6 +4224,13 @@
       <c r="F39">
         <v>18.380500000000001</v>
       </c>
+      <c r="L39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -4211,6 +4248,22 @@
       <c r="F40">
         <v>18.380500000000001</v>
       </c>
+      <c r="L40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M40" s="4"/>
+      <c r="N40" s="5">
+        <f>(M31-N31)/N31</f>
+        <v>0.11420198025618267</v>
+      </c>
+      <c r="O40" s="5">
+        <f>(M31-O31)/O31</f>
+        <v>0.13365320742694087</v>
+      </c>
+      <c r="P40" s="5">
+        <f>(M31-P31)/P31</f>
+        <v>0.1345775442192606</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -4228,6 +4281,22 @@
       <c r="F41">
         <v>18.380500000000001</v>
       </c>
+      <c r="L41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M41" s="5">
+        <f>(N31-M31)/M31</f>
+        <v>-0.10249665884629357</v>
+      </c>
+      <c r="N41" s="4"/>
+      <c r="O41" s="5">
+        <f>(N31-O31)/O31</f>
+        <v>1.7457541375295246E-2</v>
+      </c>
+      <c r="P41" s="5">
+        <f>(N31-P31)/P31</f>
+        <v>1.82871367347535E-2</v>
+      </c>
     </row>
     <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -4245,11 +4314,45 @@
       <c r="F42">
         <v>18.380500000000001</v>
       </c>
+      <c r="L42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M42" s="5">
+        <f>(O31-M31)/M31</f>
+        <v>-0.11789602547880962</v>
+      </c>
+      <c r="N42" s="5">
+        <f>(O31-N31)/N31</f>
+        <v>-1.7158004796640383E-2</v>
+      </c>
+      <c r="O42" s="4"/>
+      <c r="P42" s="5">
+        <f>(O31-P31)/P31</f>
+        <v>8.1536115830139956E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M43" s="5">
+        <f>(P31-M31)/M31</f>
+        <v>-0.1186146728400726</v>
+      </c>
+      <c r="N43" s="5">
+        <f>(P31-N31)/N31</f>
+        <v>-1.7958723109665471E-2</v>
+      </c>
+      <c r="O43" s="5">
+        <f>(P31-O31)/O31</f>
+        <v>-8.1469688610468079E-4</v>
+      </c>
+      <c r="P43" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="L34:P34"/>
+    <mergeCell ref="L39:P39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finished analysis of alphas. Created a data base of smoothed interdemand intervals
</commit_message>
<xml_diff>
--- a/bip1271_015_data.xlsx
+++ b/bip1271_015_data.xlsx
@@ -2862,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added modifications to the final manuscript of the thesis
</commit_message>
<xml_diff>
--- a/bip1271_015_data.xlsx
+++ b/bip1271_015_data.xlsx
@@ -259,11 +259,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2862,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4023,13 +4023,13 @@
       <c r="J34">
         <v>-14.94128081710544</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="L34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -4062,19 +4062,19 @@
       <c r="J35">
         <v>-12.70008869453962</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5">
+      <c r="M35" s="4"/>
+      <c r="N35" s="4">
         <f>(M32-N32)/N32</f>
         <v>8.2792442473829816E-2</v>
       </c>
-      <c r="O35" s="5">
+      <c r="O35" s="4">
         <f>(M32-O32)/O32</f>
         <v>8.422801533115841E-2</v>
       </c>
-      <c r="P35" s="5">
+      <c r="P35" s="4">
         <f>(M32-P32)/P32</f>
         <v>8.4516081833715909E-2</v>
       </c>
@@ -4110,19 +4110,19 @@
       <c r="J36">
         <v>30.204924609641321</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="4">
         <f>(N32-M32)/M32</f>
         <v>-7.6461969280720063E-2</v>
       </c>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5">
+      <c r="N36" s="4"/>
+      <c r="O36" s="4">
         <f>(N32-O32)/O32</f>
         <v>1.3258061296113018E-3</v>
       </c>
-      <c r="P36" s="5">
+      <c r="P36" s="4">
         <f>(N32-P32)/P32</f>
         <v>1.5918465000994504E-3</v>
       </c>
@@ -4158,19 +4158,19 @@
       <c r="J37">
         <v>44.674185918195121</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M37" s="4">
         <f>(O32-M32)/M32</f>
         <v>-7.7684780452230276E-2</v>
       </c>
-      <c r="N37" s="5">
+      <c r="N37" s="4">
         <f>(O32-N32)/N32</f>
         <v>-1.3240506950838436E-3</v>
       </c>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5">
+      <c r="O37" s="4"/>
+      <c r="P37" s="4">
         <f>(O32-P32)/P32</f>
         <v>2.6568811955068341E-4</v>
       </c>
@@ -4191,22 +4191,22 @@
       <c r="F38">
         <v>18.380500000000001</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M38" s="5">
+      <c r="M38" s="4">
         <f>(P32-M32)/M32</f>
         <v>-7.7929763559443824E-2</v>
       </c>
-      <c r="N38" s="5">
+      <c r="N38" s="4">
         <f>(P32-N32)/N32</f>
         <v>-1.5893165521084264E-3</v>
       </c>
-      <c r="O38" s="5">
+      <c r="O38" s="4">
         <f>(P32-O32)/O32</f>
         <v>-2.6561754812380275E-4</v>
       </c>
-      <c r="P38" s="4"/>
+      <c r="P38" s="3"/>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -4248,19 +4248,19 @@
       <c r="F40">
         <v>18.380500000000001</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="L40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="5">
+      <c r="M40" s="3"/>
+      <c r="N40" s="4">
         <f>(M31-N31)/N31</f>
         <v>0.11420198025618267</v>
       </c>
-      <c r="O40" s="5">
+      <c r="O40" s="4">
         <f>(M31-O31)/O31</f>
         <v>0.13365320742694087</v>
       </c>
-      <c r="P40" s="5">
+      <c r="P40" s="4">
         <f>(M31-P31)/P31</f>
         <v>0.1345775442192606</v>
       </c>
@@ -4281,19 +4281,19 @@
       <c r="F41">
         <v>18.380500000000001</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M41" s="4">
         <f>(N31-M31)/M31</f>
         <v>-0.10249665884629357</v>
       </c>
-      <c r="N41" s="4"/>
-      <c r="O41" s="5">
+      <c r="N41" s="3"/>
+      <c r="O41" s="4">
         <f>(N31-O31)/O31</f>
         <v>1.7457541375295246E-2</v>
       </c>
-      <c r="P41" s="5">
+      <c r="P41" s="4">
         <f>(N31-P31)/P31</f>
         <v>1.82871367347535E-2</v>
       </c>
@@ -4314,40 +4314,40 @@
       <c r="F42">
         <v>18.380500000000001</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="L42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M42" s="5">
+      <c r="M42" s="4">
         <f>(O31-M31)/M31</f>
         <v>-0.11789602547880962</v>
       </c>
-      <c r="N42" s="5">
+      <c r="N42" s="4">
         <f>(O31-N31)/N31</f>
         <v>-1.7158004796640383E-2</v>
       </c>
-      <c r="O42" s="4"/>
-      <c r="P42" s="5">
+      <c r="O42" s="3"/>
+      <c r="P42" s="4">
         <f>(O31-P31)/P31</f>
         <v>8.1536115830139956E-4</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L43" s="4" t="s">
+      <c r="L43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M43" s="5">
+      <c r="M43" s="4">
         <f>(P31-M31)/M31</f>
         <v>-0.1186146728400726</v>
       </c>
-      <c r="N43" s="5">
+      <c r="N43" s="4">
         <f>(P31-N31)/N31</f>
         <v>-1.7958723109665471E-2</v>
       </c>
-      <c r="O43" s="5">
+      <c r="O43" s="4">
         <f>(P31-O31)/O31</f>
         <v>-8.1469688610468079E-4</v>
       </c>
-      <c r="P43" s="4"/>
+      <c r="P43" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>